<commit_message>
Added state machines model
</commit_message>
<xml_diff>
--- a/TestingToolStable/Applications/C#Models/Consumer_v2/Data.xlsx
+++ b/TestingToolStable/Applications/C#Models/Consumer_v2/Data.xlsx
@@ -1,62 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="190" yWindow="520" windowWidth="28480" windowHeight="11740"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="124519"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:bookViews>
+    <x:workbookView xWindow="190" yWindow="520" windowWidth="28480" windowHeight="11740" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="124519"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-</styleSheet>
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,28 +353,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B3"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A1" sqref="A1 A1:C3"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.5"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:2"/>
+    <x:row r="2" spans="1:2"/>
+    <x:row r="3" spans="1:2"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>